<commit_message>
shift the summary title to B2 vell
</commit_message>
<xml_diff>
--- a/Final Report.xlsx
+++ b/Final Report.xlsx
@@ -42,13 +42,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -438,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A2:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +451,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Document Ageing Report</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>02.09.2025</t>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Document Ageing Report as at 02.09.2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
shift the table into B4
</commit_message>
<xml_diff>
--- a/Final Report.xlsx
+++ b/Final Report.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F46"/>
+  <dimension ref="B2:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,1153 +458,1153 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Document_currency</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Amount_in_doc_curr</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Local_Currency</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Amount_in_local_currency</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="5">
+      <c r="B5" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C5" t="n">
         <v>63010001</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>-5075015.33</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>-5075015.33</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="6">
+      <c r="B6" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C6" t="n">
         <v>63010002</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>10602307.38</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
         <v>10602307.38</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="7">
+      <c r="B7" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C7" t="n">
         <v>63010011</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>-87328000</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
         <v>-468975.88</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="B8" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C8" t="n">
         <v>63010012</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>104342390.88</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>560321.4199999999</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="B9" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C9" t="n">
         <v>63010162</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>1200328.84</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
         <v>1200328.84</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="10">
+      <c r="B10" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C10" t="n">
         <v>63010502</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>3200350.16</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
         <v>3200350.16</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="11">
+      <c r="B11" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C11" t="n">
         <v>63010512</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>-10000000</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
         <v>-53702.81</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="12">
+      <c r="B12" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C12" t="n">
         <v>63020002</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>10096056</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
         <v>54218.67000000001</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="13">
+      <c r="B13" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C13" t="n">
         <v>63020022</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>1843.75</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
         <v>1843.75</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="B14" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C14" t="n">
         <v>63020601</v>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
         <v>-5000000</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
         <v>-26851.4</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="15">
+      <c r="B15" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C15" t="n">
         <v>63020602</v>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>1058446.5</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>5684.16</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="16">
+      <c r="B16" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C16" t="n">
         <v>63010001</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>-1940771.46</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
         <v>-1940771.46</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="B17" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C17" t="n">
         <v>63010002</v>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>4162651.11</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
         <v>4162651.11</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="18">
+      <c r="B18" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C18" t="n">
         <v>63010011</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
         <v>-776102967.9299999</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
         <v>-4167890.91</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="19">
+      <c r="B19" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C19" t="n">
         <v>63010012</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>750381525.09</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
         <v>4029172.38</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="20">
+      <c r="B20" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C20" t="n">
         <v>63010502</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>1283177.49</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
         <v>1283177.49</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="21">
+      <c r="B21" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C21" t="n">
         <v>63020001</v>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>-5249772.24</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
         <v>-28192.76</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="22">
+      <c r="B22" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C22" t="n">
         <v>63020002</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>6732115.42</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
         <v>36153.37</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="23">
+      <c r="B23" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C23" t="n">
         <v>63020022</v>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>-15000000</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
         <v>-80554.21000000001</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="B24" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C24" t="n">
         <v>63020022</v>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
         <v>40</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="25">
+      <c r="B25" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C25" t="n">
         <v>63020601</v>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>-300</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
         <v>-1.61</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="B26" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="C26" t="n">
         <v>63020602</v>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
         <v>13304303.16</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
         <v>71447.85000000001</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="27">
+      <c r="B27" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="C27" t="n">
         <v>63020621</v>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>-4375</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
         <v>-4375</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="28">
+      <c r="B28" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="C28" t="n">
         <v>63070012</v>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
         <v>250851.46</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
         <v>250851.46</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="29">
+      <c r="B29" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="C29" t="n">
         <v>63070501</v>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>-389064221.27</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
         <v>-2089384.14</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="30">
+      <c r="B30" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="C30" t="n">
         <v>63070502</v>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
         <v>551275903.51</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
         <v>2960506.45</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="31">
+      <c r="B31" t="inlineStr">
         <is>
           <t>UN0151</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="C31" t="n">
         <v>63020001</v>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
         <v>127435</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
         <v>684.37</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="32">
+      <c r="B32" t="inlineStr">
         <is>
           <t>UN0151</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="C32" t="n">
         <v>63020002</v>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
         <v>-1915567</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
         <v>-10287.13</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
         <v>63010001</v>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
         <v>-6255768.25</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
         <v>-6255768.25</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
         <v>63010002</v>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
         <v>10138536.65</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
         <v>10138536.65</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
         <v>63010011</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
         <v>-1411025223.89</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
         <v>-7577601.72</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
         <v>63010012</v>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
         <v>1349137385.21</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
         <v>7244961.04</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
         <v>63010061</v>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>HKD</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="E37" t="n">
         <v>-1800000</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
         <v>-232183.17</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
         <v>63010101</v>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="E38" t="n">
         <v>-50029.99</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
         <v>-55688.38</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
         <v>63011001</v>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
         <v>-1006397.46</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
         <v>-1006397.46</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
         <v>63011011</v>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
         <v>-240245452.54</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
         <v>-1290185.31</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
         <v>63020001</v>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
         <v>-4382348.73</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
         <v>-23534.43</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
         <v>63020002</v>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
         <v>4928861.55</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
         <v>26469.37</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
         <v>63020011</v>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
         <v>-65000000</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
         <v>-349068.26</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
         <v>63020051</v>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
         <v>-35363469.34</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
         <v>-189911.76</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
         <v>63070001</v>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
         <v>-3658218.2</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
         <v>-3658218.2</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
         <v>63070002</v>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
         <v>4308857.31</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
         <v>4308857.31</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="47">
+      <c r="B47" t="inlineStr">
         <is>
           <t>XT0151</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="C47" t="n">
         <v>63020001</v>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
         <v>2785</v>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
         <v>14.92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add light blue colur for the table header
</commit_message>
<xml_diff>
--- a/Final Report.xlsx
+++ b/Final Report.xlsx
@@ -55,12 +55,18 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,9 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -459,32 +466,32 @@
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>Document_currency</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Amount_in_doc_curr</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Local_Currency</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Amount_in_local_currency</t>
         </is>

</xml_diff>

<commit_message>
add test data row
</commit_message>
<xml_diff>
--- a/Final Report.xlsx
+++ b/Final Report.xlsx
@@ -69,7 +69,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,14 +77,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -450,14 +457,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:G47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="2" customWidth="1" min="1" max="1"/>
+    <col width="41" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
         <is>
@@ -498,1120 +510,1120 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="3" t="n">
         <v>63010001</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
         <v>-5075015.33</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>-5075015.33</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="3" t="n">
         <v>63010002</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
         <v>10602307.38</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>10602307.38</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="3" t="n">
         <v>63010011</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
         <v>-87328000</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>-468975.88</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="3" t="n">
         <v>63010012</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
         <v>104342390.88</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="n">
         <v>560321.4199999999</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="3" t="n">
         <v>63010162</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
         <v>1200328.84</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="n">
         <v>1200328.84</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="3" t="n">
         <v>63010502</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
         <v>3200350.16</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="n">
         <v>3200350.16</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="3" t="n">
         <v>63010512</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
         <v>-10000000</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="n">
         <v>-53702.81</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="3" t="n">
         <v>63020002</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="n">
         <v>10096056</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="n">
         <v>54218.67000000001</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="3" t="n">
         <v>63020022</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="n">
         <v>1843.75</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="n">
         <v>1843.75</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="3" t="n">
         <v>63020601</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="n">
         <v>-5000000</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="n">
         <v>-26851.4</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
         <is>
           <t>UN0100</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="3" t="n">
         <v>63020602</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="n">
         <v>1058446.5</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="n">
         <v>5684.16</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="3" t="n">
         <v>63010001</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="n">
         <v>-1940771.46</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="n">
         <v>-1940771.46</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="3" t="n">
         <v>63010002</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="n">
         <v>4162651.11</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="n">
         <v>4162651.11</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="3" t="n">
         <v>63010011</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="n">
         <v>-776102967.9299999</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="n">
         <v>-4167890.91</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="3" t="n">
         <v>63010012</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="n">
         <v>750381525.09</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="n">
         <v>4029172.38</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="3" t="n">
         <v>63010502</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="n">
         <v>1283177.49</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="n">
         <v>1283177.49</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="3" t="n">
         <v>63020001</v>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="n">
         <v>-5249772.24</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="n">
         <v>-28192.76</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="3" t="n">
         <v>63020002</v>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="n">
         <v>6732115.42</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="n">
         <v>36153.37</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="3" t="n">
         <v>63020022</v>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="n">
         <v>-15000000</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="n">
         <v>-80554.21000000001</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="3" t="n">
         <v>63020022</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="3" t="n">
         <v>63020601</v>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="n">
         <v>-300</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="n">
         <v>-1.61</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="3" t="n">
         <v>63020602</v>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E26" s="3" t="n">
         <v>13304303.16</v>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="n">
         <v>71447.85000000001</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="3" t="n">
         <v>63020621</v>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="n">
         <v>-4375</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="n">
         <v>-4375</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="3" t="n">
         <v>63070012</v>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="n">
         <v>250851.46</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="n">
         <v>250851.46</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="3" t="n">
         <v>63070501</v>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E29" s="3" t="n">
         <v>-389064221.27</v>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="n">
         <v>-2089384.14</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="3" t="inlineStr">
         <is>
           <t>UN0150</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="3" t="n">
         <v>63070502</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="n">
         <v>551275903.51</v>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="n">
         <v>2960506.45</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="3" t="inlineStr">
         <is>
           <t>UN0151</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="3" t="n">
         <v>63020001</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="n">
         <v>127435</v>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G31" s="3" t="n">
         <v>684.37</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="3" t="inlineStr">
         <is>
           <t>UN0151</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="3" t="n">
         <v>63020002</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="n">
         <v>-1915567</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="n">
         <v>-10287.13</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n">
         <v>63010001</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="n">
         <v>-6255768.25</v>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="n">
         <v>-6255768.25</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="n">
         <v>63010002</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="n">
         <v>10138536.65</v>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="n">
         <v>10138536.65</v>
       </c>
     </row>
     <row r="35">
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n">
         <v>63010011</v>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E35" s="3" t="n">
         <v>-1411025223.89</v>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="n">
         <v>-7577601.72</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n">
         <v>63010012</v>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="n">
         <v>1349137385.21</v>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="n">
         <v>7244961.04</v>
       </c>
     </row>
     <row r="37">
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
         <v>63010061</v>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="3" t="inlineStr">
         <is>
           <t>HKD</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" s="3" t="n">
         <v>-1800000</v>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G37" s="3" t="n">
         <v>-232183.17</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
         <v>63010101</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="3" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" s="3" t="n">
         <v>-50029.99</v>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G38" s="3" t="n">
         <v>-55688.38</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
         <v>63011001</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="n">
         <v>-1006397.46</v>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="n">
         <v>-1006397.46</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n">
         <v>63011011</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="n">
         <v>-240245452.54</v>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="n">
         <v>-1290185.31</v>
       </c>
     </row>
     <row r="41">
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="n">
         <v>63020001</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="n">
         <v>-4382348.73</v>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G41" t="n">
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="n">
         <v>-23534.43</v>
       </c>
     </row>
     <row r="42">
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="n">
         <v>63020002</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="n">
         <v>4928861.55</v>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="n">
         <v>26469.37</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n">
         <v>63020011</v>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="n">
         <v>-65000000</v>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="n">
         <v>-349068.26</v>
       </c>
     </row>
     <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n">
         <v>63020051</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="n">
         <v>-35363469.34</v>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="n">
         <v>-189911.76</v>
       </c>
     </row>
     <row r="45">
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n">
         <v>63070001</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="n">
         <v>-3658218.2</v>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="n">
         <v>-3658218.2</v>
       </c>
     </row>
     <row r="46">
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>XT0150</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n">
         <v>63070002</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="n">
         <v>4308857.31</v>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="n">
         <v>4308857.31</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="3" t="inlineStr">
         <is>
           <t>XT0151</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="3" t="n">
         <v>63020001</v>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>LKR</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="n">
         <v>2785</v>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="n">
         <v>14.92</v>
       </c>
     </row>

</xml_diff>